<commit_message>
update analysis plan with done status on report that I finnaly finished yeee
</commit_message>
<xml_diff>
--- a/Analysis_plan/Analysis_plan.xlsx
+++ b/Analysis_plan/Analysis_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\PhD\PhD_webpage\Analysis_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010327DE-5298-4BB6-8764-436BFC632657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDD7B72-DF1C-4D4E-A1C5-EFA75AFF4CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13215" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -571,8 +571,8 @@
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>18</v>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -585,8 +585,8 @@
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>18</v>
+      <c r="D7" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -599,8 +599,8 @@
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>18</v>
+      <c r="D8" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -613,8 +613,8 @@
       <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>19</v>
+      <c r="D9" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update analysis plan status and add variant to gene report
</commit_message>
<xml_diff>
--- a/Analysis_plan/Analysis_plan.xlsx
+++ b/Analysis_plan/Analysis_plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\PhD\PhD_webpage\Analysis_plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\PhD\PhD_webpage\Analysis_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF19AF30-2F9D-4B20-989D-D8E891093DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C345341B-CA08-4755-8221-B602EF1C3E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="41">
   <si>
     <t>Status</t>
   </si>
@@ -126,13 +126,28 @@
     <t>Possibilities of further cohorts in USA, with non-European individuals</t>
   </si>
   <si>
-    <t>Need to draft an analysis plan</t>
-  </si>
-  <si>
     <t>Manuscript</t>
   </si>
   <si>
     <t>GWAS 'Severe' asthma</t>
+  </si>
+  <si>
+    <t>Gene prioritisation</t>
+  </si>
+  <si>
+    <t>Gene pathway analysis, protein-protein interaction, gene-variants to bring forward for in-vitro experiments</t>
+  </si>
+  <si>
+    <t>In-vitro experiments</t>
+  </si>
+  <si>
+    <t>Create hypothesis of variant-gene mechanism for in-vitro experiments</t>
+  </si>
+  <si>
+    <t>CRISPR-Cas9 experiments</t>
+  </si>
+  <si>
+    <t>Variant to gene mapping with 8 line of evidence</t>
   </si>
 </sst>
 </file>
@@ -491,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,24 +687,21 @@
         <v>21</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>30</v>
+        <v>40</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>15</v>
@@ -698,15 +710,15 @@
         <v>15</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>15</v>
@@ -715,12 +727,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>22</v>
+    <row r="15" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>15</v>
@@ -728,13 +740,14 @@
       <c r="D15" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>15</v>
@@ -748,7 +761,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>15</v>
@@ -762,7 +775,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>15</v>
@@ -776,7 +789,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>15</v>
@@ -787,10 +800,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>15</v>
@@ -801,15 +814,43 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="C23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>